<commit_message>
Updated the data to ensure numeric data type
</commit_message>
<xml_diff>
--- a/1_population_measures/data/data.xlsx
+++ b/1_population_measures/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanlu/Desktop/TA/BA - Human Science/Preliminary/1 - Population Measures/Tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanlu/Desktop/TA/BA - Human Science/Preliminary/repo/1_population_measures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE53D97C-5022-9140-A2CE-F68A120D8389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF4FC9-2F1A-B743-837F-B0D151E3D123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mortality" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>15-24</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>55-64</t>
-  </si>
-  <si>
-    <t>Age-group</t>
   </si>
   <si>
     <t>deaths</t>
@@ -576,6 +573,9 @@
   </si>
   <si>
     <t>39 per 1000 and 10 per 1000</t>
+  </si>
+  <si>
+    <t>age</t>
   </si>
 </sst>
 </file>
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,36 +1039,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1203,14 +1203,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R182"/>
   <sheetViews>
-    <sheetView topLeftCell="H11" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" customWidth="1"/>
@@ -1219,22 +1220,22 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="I2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -1257,17 +1258,17 @@
         <v>2011</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
@@ -1294,6 +1295,9 @@
       <c r="G4">
         <v>356997.54</v>
       </c>
+      <c r="I4" t="s">
+        <v>59</v>
+      </c>
       <c r="J4">
         <v>1977</v>
       </c>
@@ -1324,29 +1328,29 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="5">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2">
         <f>SUM(B4:B8)</f>
         <v>245.04</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="2">
         <f t="shared" ref="K5:L5" si="0">SUM(C4:C8)</f>
         <v>264.01</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <f t="shared" si="0"/>
         <v>177.99</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <f>SUM(E4:E8)</f>
         <v>1378304.59</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
         <f t="shared" ref="N5" si="1">SUM(F4:F8)</f>
         <v>986001.38</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="2">
         <f t="shared" ref="O5" si="2">SUM(G4:G8)</f>
         <v>1094706.1599999999</v>
       </c>
@@ -1386,29 +1390,29 @@
         <v>364288.67</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="5">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2">
         <f>SUM(B10:B18)</f>
         <v>63291.81</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="2">
         <f t="shared" ref="K6:L6" si="4">SUM(C10:C18)</f>
         <v>59446.490000000005</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <f t="shared" si="4"/>
         <v>40816.659999999996</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <f>SUM(E10:E18)</f>
         <v>2136119.19</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
         <f t="shared" ref="N6" si="5">SUM(F10:F18)</f>
         <v>1813821.4399999999</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="2">
         <f t="shared" ref="O6" si="6">SUM(G10:G18)</f>
         <v>1935671.2799999998</v>
       </c>
@@ -1427,29 +1431,29 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="5">
+        <v>16</v>
+      </c>
+      <c r="J7" s="2">
         <f>SUM(B20:B28)</f>
         <v>202546.55000000002</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="2">
         <f t="shared" ref="K7:L7" si="10">SUM(C20:C28)</f>
         <v>196218.74</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <f t="shared" si="10"/>
         <v>149688.34</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <f>SUM(E20:E28)</f>
         <v>1929861.25</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
         <f t="shared" ref="N7" si="11">SUM(F20:F28)</f>
         <v>2204981.58</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="2">
         <f t="shared" ref="O7" si="12">SUM(G20:G28)</f>
         <v>2124051.2399999998</v>
       </c>
@@ -1489,29 +1493,29 @@
         <v>373419.95</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="5">
+        <v>17</v>
+      </c>
+      <c r="J8" s="2">
         <f>SUM(B30:B38)</f>
         <v>237852.27</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="2">
         <f t="shared" ref="K8:L8" si="13">SUM(C30:C38)</f>
         <v>282106.19</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <f t="shared" si="13"/>
         <v>223639.46</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <f>SUM(E30:E38)</f>
         <v>2004319.71</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
         <f t="shared" ref="N8" si="14">SUM(F30:F38)</f>
         <v>2347927.92</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="2">
         <f t="shared" ref="O8" si="15">SUM(G30:G38)</f>
         <v>2159448.54</v>
       </c>
@@ -1530,29 +1534,29 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="5">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2">
         <f>SUM(B40:B48)</f>
         <v>115572.21999999999</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="2">
         <f t="shared" ref="K9:L9" si="16">SUM(C40:C48)</f>
         <v>182660.38999999998</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <f t="shared" si="16"/>
         <v>231686.24</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <f>SUM(E40:E48)</f>
         <v>1933440.05</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
         <f t="shared" ref="N9" si="17">SUM(F40:F48)</f>
         <v>2108220.9299999997</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="2">
         <f t="shared" ref="O9" si="18">SUM(G40:G48)</f>
         <v>2074311.38</v>
       </c>
@@ -1592,29 +1596,29 @@
         <v>369446.26</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="5">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2">
         <f>SUM(B50:B58)</f>
         <v>30251.329999999998</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="2">
         <f t="shared" ref="K10:L10" si="19">SUM(C50:C58)</f>
         <v>60546.05</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="2">
         <f t="shared" si="19"/>
         <v>129164.46</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="2">
         <f>SUM(E50:E58)</f>
         <v>1604278.1</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
         <f t="shared" ref="N10" si="20">SUM(F50:F58)</f>
         <v>1897847.75</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="2">
         <f t="shared" ref="O10" si="21">SUM(G50:G58)</f>
         <v>2091807.7000000002</v>
       </c>
@@ -1633,29 +1637,29 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="5">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2">
         <f>SUM(B60:B68)</f>
         <v>6752.7</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="2">
         <f t="shared" ref="K11:L11" si="22">SUM(C60:C68)</f>
         <v>10450.06</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="2">
         <f t="shared" si="22"/>
         <v>30605.68</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="2">
         <f>SUM(E60:E68)</f>
         <v>1557028.54</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
         <f t="shared" ref="N11" si="23">SUM(F60:F68)</f>
         <v>2059598.8199999998</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="2">
         <f t="shared" ref="O11" si="24">SUM(G60:G68)</f>
         <v>2337446.1</v>
       </c>
@@ -1695,29 +1699,29 @@
         <v>374878.11</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="5">
+        <v>21</v>
+      </c>
+      <c r="J12" s="2">
         <f>SUM(B70,B72,B74,B76,B78)</f>
         <v>517.1</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="2">
         <f t="shared" ref="K12:L12" si="25">SUM(C70,C72,C74,C76,C78)</f>
         <v>526.04</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="2">
         <f t="shared" si="25"/>
         <v>1869.1</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="2">
         <f>SUM(E70,E72,E74,E76,E78)</f>
         <v>1620499.3099999998</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <f t="shared" ref="N12" si="26">SUM(F70,F72,F74,F76,F78)</f>
         <v>1768419.77</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="2">
         <f t="shared" ref="O12" si="27">SUM(G70,G72,G74,G76,G78)</f>
         <v>2352581.89</v>
       </c>
@@ -1736,29 +1740,29 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="5">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2">
         <f>SUM(B80:B88)</f>
         <v>9</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="2">
         <f t="shared" ref="K13:L13" si="28">SUM(C80:C88)</f>
         <v>51.01</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="2">
         <f t="shared" si="28"/>
         <v>128.01</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="2">
         <f>SUM(E80:E88)</f>
         <v>1698277.17</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
         <f t="shared" ref="N13" si="29">SUM(F80:F88)</f>
         <v>1544471.67</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="2">
         <f t="shared" ref="O13" si="30">SUM(G80:G88)</f>
         <v>2077602.87</v>
       </c>
@@ -1837,7 +1841,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1943,7 +1947,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I23" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
@@ -1969,16 +1973,19 @@
         <v>422418.57</v>
       </c>
       <c r="J24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" t="s">
         <v>13</v>
       </c>
-      <c r="M24" t="s">
-        <v>14</v>
-      </c>
       <c r="P24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>59</v>
+      </c>
       <c r="J25">
         <v>1977</v>
       </c>
@@ -2030,24 +2037,24 @@
         <v>432217.75</v>
       </c>
       <c r="I26" t="s">
-        <v>27</v>
-      </c>
-      <c r="J26">
+        <v>26</v>
+      </c>
+      <c r="J26" s="2">
         <v>370.01</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <v>270.99</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>30</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="2">
         <v>591020.92999999993</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="2">
         <v>582321.25</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="2">
         <v>427913.70999999996</v>
       </c>
       <c r="P26">
@@ -2062,24 +2069,24 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>28</v>
-      </c>
-      <c r="J27">
+        <v>27</v>
+      </c>
+      <c r="J27" s="2">
         <v>34819</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
         <v>14710</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="2">
         <v>2817</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="2">
         <v>958643.62999999989</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="2">
         <v>886211.79999999981</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="2">
         <v>772922.70000000007</v>
       </c>
       <c r="P27">
@@ -2115,24 +2122,24 @@
         <v>430588.29</v>
       </c>
       <c r="I28" t="s">
-        <v>29</v>
-      </c>
-      <c r="J28">
+        <v>28</v>
+      </c>
+      <c r="J28" s="2">
         <v>171043</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="2">
         <v>84703</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="2">
         <v>17705</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="2">
         <v>882887.62000000011</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="2">
         <v>919253.47999999986</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="2">
         <v>768371.65999999992</v>
       </c>
       <c r="P28">
@@ -2147,24 +2154,24 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29">
+        <v>29</v>
+      </c>
+      <c r="J29" s="2">
         <v>142380</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="2">
         <v>142918</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="2">
         <v>60196</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="2">
         <v>692273.1</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="2">
         <v>960312.06</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="2">
         <v>906134.93</v>
       </c>
       <c r="P29">
@@ -2200,24 +2207,24 @@
         <v>430772.91</v>
       </c>
       <c r="I30" t="s">
-        <v>31</v>
-      </c>
-      <c r="J30">
+        <v>30</v>
+      </c>
+      <c r="J30" s="2">
         <v>31981</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="2">
         <v>62800</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="2">
         <v>82387</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="2">
         <v>440824.52</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="2">
         <v>918613.07</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="2">
         <v>1016100</v>
       </c>
       <c r="P30">
@@ -2232,24 +2239,24 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31">
+        <v>31</v>
+      </c>
+      <c r="J31" s="2">
         <v>10372</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="2">
         <v>12931</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="2">
         <v>30744</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="2">
         <v>452137.61</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="2">
         <v>832854.64</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="2">
         <v>916172.1</v>
       </c>
       <c r="P31">
@@ -2285,24 +2292,24 @@
         <v>433981.62</v>
       </c>
       <c r="I32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32">
+        <v>32</v>
+      </c>
+      <c r="J32" s="2">
         <v>2402</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="2">
         <v>1273</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="2">
         <v>4324</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="2">
         <v>396349.72</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="2">
         <v>596838.29</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="2">
         <v>926476.86999999988</v>
       </c>
       <c r="P32">
@@ -2317,24 +2324,24 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33">
+        <v>33</v>
+      </c>
+      <c r="J33" s="2">
         <v>194</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="2">
         <v>47</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="2">
         <v>131</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="2">
         <v>349212.81</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="2">
         <v>432532.54000000004</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="2">
         <v>953482.66</v>
       </c>
       <c r="P33">
@@ -2370,24 +2377,24 @@
         <v>427568.01</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34">
+        <v>34</v>
+      </c>
+      <c r="J34" s="2">
         <v>72.000000000000014</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="2">
         <v>27.02</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="2">
         <v>13.99</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="2">
         <v>285352.37</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="2">
         <v>428939.35</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="2">
         <v>902003.09000000008</v>
       </c>
       <c r="P34">
@@ -2434,7 +2441,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -3066,7 +3073,7 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -3089,15 +3096,15 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
@@ -3122,24 +3129,24 @@
         <v>2011</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K95" s="9"/>
       <c r="L95" s="9"/>
       <c r="M95" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N95" s="9"/>
       <c r="O95" s="9"/>
       <c r="P95" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q95" s="9"/>
       <c r="R95" s="9"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B96">
         <v>0.36</v>
@@ -3189,7 +3196,7 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J97" s="5">
         <f>SUM(B96:B100)</f>
@@ -3251,7 +3258,7 @@
         <v>141551.41</v>
       </c>
       <c r="I98" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J98" s="5">
         <f>SUM(B102:B110)</f>
@@ -3292,7 +3299,7 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I99" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J99" s="5">
         <f>SUM(B112:B120)</f>
@@ -3354,7 +3361,7 @@
         <v>154658.65</v>
       </c>
       <c r="I100" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J100" s="5">
         <f>SUM(B122:B130)</f>
@@ -3395,7 +3402,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J101" s="5">
         <f>SUM(B132:B140)</f>
@@ -3457,7 +3464,7 @@
         <v>155290.65</v>
       </c>
       <c r="I102" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J102" s="5">
         <f>SUM(B142:B150)</f>
@@ -3498,7 +3505,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I103" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J103" s="5">
         <f>SUM(B152:B160)</f>
@@ -3560,7 +3567,7 @@
         <v>155241.75</v>
       </c>
       <c r="I104" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J104" s="5">
         <f>SUM(B162,B164,B166,B168,B170)</f>
@@ -3601,7 +3608,7 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J105" s="5">
         <f>SUM(B172:B180)</f>
@@ -3665,7 +3672,7 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O107" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P107" s="4">
         <f>SUM(P98:P104)*5</f>
@@ -3703,7 +3710,7 @@
         <v>154715.84</v>
       </c>
       <c r="I108" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
@@ -3717,7 +3724,7 @@
         <v>17043000</v>
       </c>
       <c r="O109" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P109">
         <f>SUM(J97:J105)/K109*1000</f>
@@ -4582,7 +4589,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -4625,7 +4632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A13:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="103" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="103" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -4636,10 +4643,10 @@
   <sheetData>
     <row r="13" spans="10:14" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L13">
         <v>1900</v>
@@ -4667,10 +4674,10 @@
     </row>
     <row r="16" spans="10:14" x14ac:dyDescent="0.2">
       <c r="J16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L16">
         <v>1902</v>
@@ -4691,13 +4698,13 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
         <v>51</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>52</v>
-      </c>
-      <c r="M19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -4712,13 +4719,13 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="J22" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" t="s">
         <v>54</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>55</v>
-      </c>
-      <c r="M22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4733,59 +4740,59 @@
     </row>
     <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>